<commit_message>
committing before jumping back in
</commit_message>
<xml_diff>
--- a/Data/Odds/NBA/NBA odds 2020-21.xlsx
+++ b/Data/Odds/NBA/NBA odds 2020-21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2237"/>
+  <dimension ref="A1:M2343"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -101236,6 +101236,4856 @@
         <v>114.5</v>
       </c>
     </row>
+    <row r="2238">
+      <c r="A2238" t="n">
+        <v>601</v>
+      </c>
+      <c r="B2238" t="n">
+        <v>521</v>
+      </c>
+      <c r="C2238" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2238" t="inlineStr">
+        <is>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="E2238" t="n">
+        <v>24</v>
+      </c>
+      <c r="F2238" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2238" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2238" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2238" t="n">
+        <v>109</v>
+      </c>
+      <c r="J2238" t="n">
+        <v>231.5</v>
+      </c>
+      <c r="K2238" t="n">
+        <v>234.5</v>
+      </c>
+      <c r="L2238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+750 </t>
+        </is>
+      </c>
+      <c r="M2238" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2239">
+      <c r="A2239" t="n">
+        <v>601</v>
+      </c>
+      <c r="B2239" t="n">
+        <v>522</v>
+      </c>
+      <c r="C2239" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2239" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2239" t="n">
+        <v>31</v>
+      </c>
+      <c r="F2239" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2239" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2239" t="n">
+        <v>37</v>
+      </c>
+      <c r="I2239" t="n">
+        <v>123</v>
+      </c>
+      <c r="J2239" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="K2239" t="n">
+        <v>13</v>
+      </c>
+      <c r="L2239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-1200 </t>
+        </is>
+      </c>
+      <c r="M2239" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="2240">
+      <c r="A2240" t="n">
+        <v>601</v>
+      </c>
+      <c r="B2240" t="n">
+        <v>523</v>
+      </c>
+      <c r="C2240" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2240" t="inlineStr">
+        <is>
+          <t>Portland</t>
+        </is>
+      </c>
+      <c r="E2240" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2240" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2240" t="n">
+        <v>32</v>
+      </c>
+      <c r="H2240" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2240" t="n">
+        <v>140</v>
+      </c>
+      <c r="J2240" t="n">
+        <v>226</v>
+      </c>
+      <c r="K2240" t="n">
+        <v>226.5</v>
+      </c>
+      <c r="L2240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+115 </t>
+        </is>
+      </c>
+      <c r="M2240" t="n">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="2241">
+      <c r="A2241" t="n">
+        <v>601</v>
+      </c>
+      <c r="B2241" t="n">
+        <v>524</v>
+      </c>
+      <c r="C2241" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2241" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E2241" t="n">
+        <v>38</v>
+      </c>
+      <c r="F2241" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2241" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2241" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2241" t="n">
+        <v>147</v>
+      </c>
+      <c r="J2241" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K2241" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-135 </t>
+        </is>
+      </c>
+      <c r="M2241" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2242">
+      <c r="A2242" t="n">
+        <v>601</v>
+      </c>
+      <c r="B2242" t="n">
+        <v>525</v>
+      </c>
+      <c r="C2242" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2242" t="inlineStr">
+        <is>
+          <t>LALakers</t>
+        </is>
+      </c>
+      <c r="E2242" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2242" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2242" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2242" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2242" t="n">
+        <v>85</v>
+      </c>
+      <c r="J2242" t="n">
+        <v>209.5</v>
+      </c>
+      <c r="K2242" t="n">
+        <v>209.5</v>
+      </c>
+      <c r="L2242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+175 </t>
+        </is>
+      </c>
+      <c r="M2242" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="2243">
+      <c r="A2243" t="n">
+        <v>601</v>
+      </c>
+      <c r="B2243" t="n">
+        <v>526</v>
+      </c>
+      <c r="C2243" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2243" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2243" t="n">
+        <v>34</v>
+      </c>
+      <c r="F2243" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2243" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2243" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2243" t="n">
+        <v>115</v>
+      </c>
+      <c r="J2243" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2243" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-200 </t>
+        </is>
+      </c>
+      <c r="M2243" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2244">
+      <c r="A2244" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2244" t="n">
+        <v>531</v>
+      </c>
+      <c r="C2244" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2244" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2244" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2244" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2244" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2244" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2244" t="n">
+        <v>103</v>
+      </c>
+      <c r="J2244" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="K2244" t="n">
+        <v>209</v>
+      </c>
+      <c r="L2244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+100 </t>
+        </is>
+      </c>
+      <c r="M2244" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2245">
+      <c r="A2245" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2245" t="n">
+        <v>532</v>
+      </c>
+      <c r="C2245" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2245" t="inlineStr">
+        <is>
+          <t>NewYork</t>
+        </is>
+      </c>
+      <c r="E2245" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2245" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2245" t="n">
+        <v>15</v>
+      </c>
+      <c r="H2245" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2245" t="n">
+        <v>89</v>
+      </c>
+      <c r="J2245" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K2245" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-120 </t>
+        </is>
+      </c>
+      <c r="M2245" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="2246">
+      <c r="A2246" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2246" t="n">
+        <v>533</v>
+      </c>
+      <c r="C2246" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2246" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E2246" t="n">
+        <v>35</v>
+      </c>
+      <c r="F2246" t="n">
+        <v>21</v>
+      </c>
+      <c r="G2246" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2246" t="n">
+        <v>16</v>
+      </c>
+      <c r="I2246" t="n">
+        <v>105</v>
+      </c>
+      <c r="J2246" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="K2246" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="L2246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+280 </t>
+        </is>
+      </c>
+      <c r="M2246" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2247">
+      <c r="A2247" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2247" t="n">
+        <v>534</v>
+      </c>
+      <c r="C2247" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2247" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2247" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2247" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2247" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2247" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2247" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2247" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2247" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L2247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-340 </t>
+        </is>
+      </c>
+      <c r="M2247" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2248">
+      <c r="A2248" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2248" t="n">
+        <v>535</v>
+      </c>
+      <c r="C2248" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2248" t="inlineStr">
+        <is>
+          <t>Memphis</t>
+        </is>
+      </c>
+      <c r="E2248" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2248" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2248" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2248" t="n">
+        <v>34</v>
+      </c>
+      <c r="I2248" t="n">
+        <v>110</v>
+      </c>
+      <c r="J2248" t="n">
+        <v>226</v>
+      </c>
+      <c r="K2248" t="n">
+        <v>226.5</v>
+      </c>
+      <c r="L2248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+380 </t>
+        </is>
+      </c>
+      <c r="M2248" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2249">
+      <c r="A2249" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2249" t="n">
+        <v>536</v>
+      </c>
+      <c r="C2249" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2249" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2249" t="n">
+        <v>47</v>
+      </c>
+      <c r="F2249" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2249" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2249" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2249" t="n">
+        <v>126</v>
+      </c>
+      <c r="J2249" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="K2249" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L2249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-460 </t>
+        </is>
+      </c>
+      <c r="M2249" t="n">
+        <v>115.5</v>
+      </c>
+    </row>
+    <row r="2250">
+      <c r="A2250" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2250" t="n">
+        <v>537</v>
+      </c>
+      <c r="C2250" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2250" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E2250" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2250" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2250" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2250" t="n">
+        <v>18</v>
+      </c>
+      <c r="I2250" t="n">
+        <v>112</v>
+      </c>
+      <c r="J2250" t="n">
+        <v>230.5</v>
+      </c>
+      <c r="K2250" t="n">
+        <v>229</v>
+      </c>
+      <c r="L2250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+210 </t>
+        </is>
+      </c>
+      <c r="M2250" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2251">
+      <c r="A2251" t="n">
+        <v>602</v>
+      </c>
+      <c r="B2251" t="n">
+        <v>538</v>
+      </c>
+      <c r="C2251" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2251" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2251" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2251" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2251" t="n">
+        <v>38</v>
+      </c>
+      <c r="H2251" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2251" t="n">
+        <v>129</v>
+      </c>
+      <c r="J2251" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K2251" t="n">
+        <v>6</v>
+      </c>
+      <c r="L2251" t="n">
+        <v>-250</v>
+      </c>
+      <c r="M2251" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2252">
+      <c r="A2252" t="n">
+        <v>603</v>
+      </c>
+      <c r="B2252" t="n">
+        <v>543</v>
+      </c>
+      <c r="C2252" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2252" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2252" t="n">
+        <v>36</v>
+      </c>
+      <c r="F2252" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2252" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2252" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2252" t="n">
+        <v>113</v>
+      </c>
+      <c r="J2252" t="n">
+        <v>208.5</v>
+      </c>
+      <c r="K2252" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="L2252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+120 </t>
+        </is>
+      </c>
+      <c r="M2252" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2253">
+      <c r="A2253" t="n">
+        <v>603</v>
+      </c>
+      <c r="B2253" t="n">
+        <v>544</v>
+      </c>
+      <c r="C2253" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2253" t="inlineStr">
+        <is>
+          <t>LALakers</t>
+        </is>
+      </c>
+      <c r="E2253" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2253" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2253" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2253" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2253" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2253" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2253" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-140 </t>
+        </is>
+      </c>
+      <c r="M2253" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2254">
+      <c r="A2254" t="n">
+        <v>603</v>
+      </c>
+      <c r="B2254" t="n">
+        <v>545</v>
+      </c>
+      <c r="C2254" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2254" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E2254" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2254" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2254" t="n">
+        <v>37</v>
+      </c>
+      <c r="H2254" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2254" t="n">
+        <v>126</v>
+      </c>
+      <c r="J2254" t="n">
+        <v>228.5</v>
+      </c>
+      <c r="K2254" t="n">
+        <v>228</v>
+      </c>
+      <c r="L2254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+175 </t>
+        </is>
+      </c>
+      <c r="M2254" t="n">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="2255">
+      <c r="A2255" t="n">
+        <v>603</v>
+      </c>
+      <c r="B2255" t="n">
+        <v>546</v>
+      </c>
+      <c r="C2255" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2255" t="inlineStr">
+        <is>
+          <t>Portland</t>
+        </is>
+      </c>
+      <c r="E2255" t="n">
+        <v>33</v>
+      </c>
+      <c r="F2255" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2255" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2255" t="n">
+        <v>14</v>
+      </c>
+      <c r="I2255" t="n">
+        <v>115</v>
+      </c>
+      <c r="J2255" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2255" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2255" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M2255" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2256">
+      <c r="A2256" t="n">
+        <v>604</v>
+      </c>
+      <c r="B2256" t="n">
+        <v>557</v>
+      </c>
+      <c r="C2256" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2256" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2256" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2256" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2256" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2256" t="n">
+        <v>31</v>
+      </c>
+      <c r="I2256" t="n">
+        <v>104</v>
+      </c>
+      <c r="J2256" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2256" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-145 </t>
+        </is>
+      </c>
+      <c r="M2256" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2257">
+      <c r="A2257" t="n">
+        <v>604</v>
+      </c>
+      <c r="B2257" t="n">
+        <v>558</v>
+      </c>
+      <c r="C2257" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2257" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E2257" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2257" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2257" t="n">
+        <v>32</v>
+      </c>
+      <c r="H2257" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2257" t="n">
+        <v>97</v>
+      </c>
+      <c r="J2257" t="n">
+        <v>216.5</v>
+      </c>
+      <c r="K2257" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="L2257" t="n">
+        <v>125</v>
+      </c>
+      <c r="M2257" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2258">
+      <c r="A2258" t="n">
+        <v>605</v>
+      </c>
+      <c r="B2258" t="n">
+        <v>561</v>
+      </c>
+      <c r="C2258" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2258" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2258" t="n">
+        <v>32</v>
+      </c>
+      <c r="F2258" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2258" t="n">
+        <v>23</v>
+      </c>
+      <c r="H2258" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2258" t="n">
+        <v>107</v>
+      </c>
+      <c r="J2258" t="n">
+        <v>240</v>
+      </c>
+      <c r="K2258" t="n">
+        <v>239.5</v>
+      </c>
+      <c r="L2258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+145 </t>
+        </is>
+      </c>
+      <c r="M2258" t="n">
+        <v>120.5</v>
+      </c>
+    </row>
+    <row r="2259">
+      <c r="A2259" t="n">
+        <v>605</v>
+      </c>
+      <c r="B2259" t="n">
+        <v>562</v>
+      </c>
+      <c r="C2259" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2259" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2259" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2259" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2259" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2259" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2259" t="n">
+        <v>115</v>
+      </c>
+      <c r="J2259" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2259" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2259" t="n">
+        <v>-165</v>
+      </c>
+      <c r="M2259" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2260">
+      <c r="A2260" t="n">
+        <v>606</v>
+      </c>
+      <c r="B2260" t="n">
+        <v>571</v>
+      </c>
+      <c r="C2260" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2260" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2260" t="n">
+        <v>42</v>
+      </c>
+      <c r="F2260" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2260" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2260" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2260" t="n">
+        <v>128</v>
+      </c>
+      <c r="J2260" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="K2260" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="L2260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+170 </t>
+        </is>
+      </c>
+      <c r="M2260" t="n">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="2261">
+      <c r="A2261" t="n">
+        <v>606</v>
+      </c>
+      <c r="B2261" t="n">
+        <v>572</v>
+      </c>
+      <c r="C2261" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2261" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2261" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2261" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2261" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2261" t="n">
+        <v>41</v>
+      </c>
+      <c r="I2261" t="n">
+        <v>124</v>
+      </c>
+      <c r="J2261" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K2261" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-190 </t>
+        </is>
+      </c>
+      <c r="M2261" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="2262">
+      <c r="A2262" t="n">
+        <v>606</v>
+      </c>
+      <c r="B2262" t="n">
+        <v>573</v>
+      </c>
+      <c r="C2262" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2262" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E2262" t="n">
+        <v>38</v>
+      </c>
+      <c r="F2262" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2262" t="n">
+        <v>23</v>
+      </c>
+      <c r="H2262" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2262" t="n">
+        <v>111</v>
+      </c>
+      <c r="J2262" t="n">
+        <v>214.5</v>
+      </c>
+      <c r="K2262" t="n">
+        <v>211.5</v>
+      </c>
+      <c r="L2262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+225 </t>
+        </is>
+      </c>
+      <c r="M2262" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2263">
+      <c r="A2263" t="n">
+        <v>606</v>
+      </c>
+      <c r="B2263" t="n">
+        <v>574</v>
+      </c>
+      <c r="C2263" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2263" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2263" t="n">
+        <v>35</v>
+      </c>
+      <c r="F2263" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2263" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2263" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2263" t="n">
+        <v>126</v>
+      </c>
+      <c r="J2263" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K2263" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="L2263" t="n">
+        <v>-265</v>
+      </c>
+      <c r="M2263" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2264">
+      <c r="A2264" t="n">
+        <v>607</v>
+      </c>
+      <c r="B2264" t="n">
+        <v>581</v>
+      </c>
+      <c r="C2264" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2264" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2264" t="n">
+        <v>19</v>
+      </c>
+      <c r="F2264" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2264" t="n">
+        <v>24</v>
+      </c>
+      <c r="H2264" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2264" t="n">
+        <v>86</v>
+      </c>
+      <c r="J2264" t="n">
+        <v>235</v>
+      </c>
+      <c r="K2264" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L2264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-135 </t>
+        </is>
+      </c>
+      <c r="M2264" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="2265">
+      <c r="A2265" t="n">
+        <v>607</v>
+      </c>
+      <c r="B2265" t="n">
+        <v>582</v>
+      </c>
+      <c r="C2265" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2265" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2265" t="n">
+        <v>36</v>
+      </c>
+      <c r="F2265" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2265" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2265" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2265" t="n">
+        <v>125</v>
+      </c>
+      <c r="J2265" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2265" t="n">
+        <v>238</v>
+      </c>
+      <c r="L2265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+115 </t>
+        </is>
+      </c>
+      <c r="M2265" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2266">
+      <c r="A2266" t="n">
+        <v>607</v>
+      </c>
+      <c r="B2266" t="n">
+        <v>583</v>
+      </c>
+      <c r="C2266" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2266" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E2266" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2266" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2266" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2266" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2266" t="n">
+        <v>105</v>
+      </c>
+      <c r="J2266" t="n">
+        <v>220</v>
+      </c>
+      <c r="K2266" t="n">
+        <v>222</v>
+      </c>
+      <c r="L2266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+190 </t>
+        </is>
+      </c>
+      <c r="M2266" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="2267">
+      <c r="A2267" t="n">
+        <v>607</v>
+      </c>
+      <c r="B2267" t="n">
+        <v>584</v>
+      </c>
+      <c r="C2267" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2267" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2267" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2267" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2267" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2267" t="n">
+        <v>34</v>
+      </c>
+      <c r="I2267" t="n">
+        <v>122</v>
+      </c>
+      <c r="J2267" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K2267" t="n">
+        <v>6</v>
+      </c>
+      <c r="L2267" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M2267" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="2268">
+      <c r="A2268" t="n">
+        <v>608</v>
+      </c>
+      <c r="B2268" t="n">
+        <v>501</v>
+      </c>
+      <c r="C2268" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2268" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2268" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2268" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2268" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2268" t="n">
+        <v>18</v>
+      </c>
+      <c r="I2268" t="n">
+        <v>102</v>
+      </c>
+      <c r="J2268" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="K2268" t="n">
+        <v>225.5</v>
+      </c>
+      <c r="L2268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+240 </t>
+        </is>
+      </c>
+      <c r="M2268" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2269">
+      <c r="A2269" t="n">
+        <v>608</v>
+      </c>
+      <c r="B2269" t="n">
+        <v>502</v>
+      </c>
+      <c r="C2269" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2269" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2269" t="n">
+        <v>33</v>
+      </c>
+      <c r="F2269" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2269" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2269" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2269" t="n">
+        <v>118</v>
+      </c>
+      <c r="J2269" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2269" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="L2269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-280 </t>
+        </is>
+      </c>
+      <c r="M2269" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2270">
+      <c r="A2270" t="n">
+        <v>608</v>
+      </c>
+      <c r="B2270" t="n">
+        <v>503</v>
+      </c>
+      <c r="C2270" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2270" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2270" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2270" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2270" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2270" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2270" t="n">
+        <v>109</v>
+      </c>
+      <c r="J2270" t="n">
+        <v>221.5</v>
+      </c>
+      <c r="K2270" t="n">
+        <v>222</v>
+      </c>
+      <c r="L2270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+130 </t>
+        </is>
+      </c>
+      <c r="M2270" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2271">
+      <c r="A2271" t="n">
+        <v>608</v>
+      </c>
+      <c r="B2271" t="n">
+        <v>504</v>
+      </c>
+      <c r="C2271" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2271" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2271" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2271" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2271" t="n">
+        <v>32</v>
+      </c>
+      <c r="H2271" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2271" t="n">
+        <v>112</v>
+      </c>
+      <c r="J2271" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2271" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2271" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M2271" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2272">
+      <c r="A2272" t="n">
+        <v>609</v>
+      </c>
+      <c r="B2272" t="n">
+        <v>511</v>
+      </c>
+      <c r="C2272" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2272" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E2272" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2272" t="n">
+        <v>21</v>
+      </c>
+      <c r="G2272" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2272" t="n">
+        <v>31</v>
+      </c>
+      <c r="I2272" t="n">
+        <v>98</v>
+      </c>
+      <c r="J2272" t="n">
+        <v>221</v>
+      </c>
+      <c r="K2272" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="L2272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+180 </t>
+        </is>
+      </c>
+      <c r="M2272" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2273">
+      <c r="A2273" t="n">
+        <v>609</v>
+      </c>
+      <c r="B2273" t="n">
+        <v>512</v>
+      </c>
+      <c r="C2273" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2273" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2273" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2273" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2273" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2273" t="n">
+        <v>37</v>
+      </c>
+      <c r="I2273" t="n">
+        <v>123</v>
+      </c>
+      <c r="J2273" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2273" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L2273" t="n">
+        <v>-210</v>
+      </c>
+      <c r="M2273" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="2274">
+      <c r="A2274" t="n">
+        <v>610</v>
+      </c>
+      <c r="B2274" t="n">
+        <v>521</v>
+      </c>
+      <c r="C2274" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2274" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2274" t="n">
+        <v>11</v>
+      </c>
+      <c r="F2274" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2274" t="n">
+        <v>23</v>
+      </c>
+      <c r="H2274" t="n">
+        <v>18</v>
+      </c>
+      <c r="I2274" t="n">
+        <v>83</v>
+      </c>
+      <c r="J2274" t="n">
+        <v>234</v>
+      </c>
+      <c r="K2274" t="n">
+        <v>235</v>
+      </c>
+      <c r="L2274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+140 </t>
+        </is>
+      </c>
+      <c r="M2274" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2275">
+      <c r="A2275" t="n">
+        <v>610</v>
+      </c>
+      <c r="B2275" t="n">
+        <v>522</v>
+      </c>
+      <c r="C2275" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2275" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2275" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2275" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2275" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2275" t="n">
+        <v>19</v>
+      </c>
+      <c r="I2275" t="n">
+        <v>86</v>
+      </c>
+      <c r="J2275" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2275" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L2275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-160 </t>
+        </is>
+      </c>
+      <c r="M2275" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2276">
+      <c r="A2276" t="n">
+        <v>610</v>
+      </c>
+      <c r="B2276" t="n">
+        <v>523</v>
+      </c>
+      <c r="C2276" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2276" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2276" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2276" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2276" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2276" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2276" t="n">
+        <v>111</v>
+      </c>
+      <c r="J2276" t="n">
+        <v>221</v>
+      </c>
+      <c r="K2276" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="L2276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+120 </t>
+        </is>
+      </c>
+      <c r="M2276" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2277">
+      <c r="A2277" t="n">
+        <v>610</v>
+      </c>
+      <c r="B2277" t="n">
+        <v>524</v>
+      </c>
+      <c r="C2277" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2277" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2277" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2277" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2277" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2277" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2277" t="n">
+        <v>117</v>
+      </c>
+      <c r="J2277" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2277" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L2277" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M2277" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="2278">
+      <c r="A2278" t="n">
+        <v>611</v>
+      </c>
+      <c r="B2278" t="n">
+        <v>531</v>
+      </c>
+      <c r="C2278" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2278" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2278" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2278" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2278" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2278" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2278" t="n">
+        <v>127</v>
+      </c>
+      <c r="J2278" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2278" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-130 </t>
+        </is>
+      </c>
+      <c r="M2278" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2279">
+      <c r="A2279" t="n">
+        <v>611</v>
+      </c>
+      <c r="B2279" t="n">
+        <v>532</v>
+      </c>
+      <c r="C2279" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2279" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2279" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2279" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2279" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2279" t="n">
+        <v>36</v>
+      </c>
+      <c r="I2279" t="n">
+        <v>111</v>
+      </c>
+      <c r="J2279" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="K2279" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="L2279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+110 </t>
+        </is>
+      </c>
+      <c r="M2279" t="n">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="2280">
+      <c r="A2280" t="n">
+        <v>611</v>
+      </c>
+      <c r="B2280" t="n">
+        <v>533</v>
+      </c>
+      <c r="C2280" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2280" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2280" t="n">
+        <v>37</v>
+      </c>
+      <c r="F2280" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2280" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2280" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2280" t="n">
+        <v>116</v>
+      </c>
+      <c r="J2280" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="K2280" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="L2280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+110 </t>
+        </is>
+      </c>
+      <c r="M2280" t="n">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="2281">
+      <c r="A2281" t="n">
+        <v>611</v>
+      </c>
+      <c r="B2281" t="n">
+        <v>534</v>
+      </c>
+      <c r="C2281" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2281" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E2281" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2281" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2281" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2281" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2281" t="n">
+        <v>102</v>
+      </c>
+      <c r="J2281" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K2281" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2281" t="n">
+        <v>-130</v>
+      </c>
+      <c r="M2281" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2282">
+      <c r="A2282" t="n">
+        <v>612</v>
+      </c>
+      <c r="B2282" t="n">
+        <v>541</v>
+      </c>
+      <c r="C2282" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2282" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2282" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2282" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2282" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2282" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2282" t="n">
+        <v>106</v>
+      </c>
+      <c r="J2282" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="K2282" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="L2282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+175 </t>
+        </is>
+      </c>
+      <c r="M2282" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2283">
+      <c r="A2283" t="n">
+        <v>612</v>
+      </c>
+      <c r="B2283" t="n">
+        <v>542</v>
+      </c>
+      <c r="C2283" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2283" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2283" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2283" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2283" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2283" t="n">
+        <v>38</v>
+      </c>
+      <c r="I2283" t="n">
+        <v>132</v>
+      </c>
+      <c r="J2283" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2283" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2283" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M2283" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2284">
+      <c r="A2284" t="n">
+        <v>613</v>
+      </c>
+      <c r="B2284" t="n">
+        <v>551</v>
+      </c>
+      <c r="C2284" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2284" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2284" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2284" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2284" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2284" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2284" t="n">
+        <v>96</v>
+      </c>
+      <c r="J2284" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2284" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2284" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-135 </t>
+        </is>
+      </c>
+      <c r="M2284" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2285">
+      <c r="A2285" t="n">
+        <v>613</v>
+      </c>
+      <c r="B2285" t="n">
+        <v>552</v>
+      </c>
+      <c r="C2285" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2285" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2285" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2285" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2285" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2285" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2285" t="n">
+        <v>107</v>
+      </c>
+      <c r="J2285" t="n">
+        <v>230</v>
+      </c>
+      <c r="K2285" t="n">
+        <v>228.5</v>
+      </c>
+      <c r="L2285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+115 </t>
+        </is>
+      </c>
+      <c r="M2285" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2286">
+      <c r="A2286" t="n">
+        <v>613</v>
+      </c>
+      <c r="B2286" t="n">
+        <v>553</v>
+      </c>
+      <c r="C2286" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2286" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2286" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2286" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2286" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2286" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2286" t="n">
+        <v>125</v>
+      </c>
+      <c r="J2286" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K2286" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">-155 </t>
+        </is>
+      </c>
+      <c r="M2286" t="n">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="2287">
+      <c r="A2287" t="n">
+        <v>613</v>
+      </c>
+      <c r="B2287" t="n">
+        <v>554</v>
+      </c>
+      <c r="C2287" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2287" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E2287" t="n">
+        <v>22</v>
+      </c>
+      <c r="F2287" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2287" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2287" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2287" t="n">
+        <v>118</v>
+      </c>
+      <c r="J2287" t="n">
+        <v>221</v>
+      </c>
+      <c r="K2287" t="n">
+        <v>223</v>
+      </c>
+      <c r="L2287" t="n">
+        <v>135</v>
+      </c>
+      <c r="M2287" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2288">
+      <c r="A2288" t="n">
+        <v>614</v>
+      </c>
+      <c r="B2288" t="n">
+        <v>561</v>
+      </c>
+      <c r="C2288" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2288" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2288" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2288" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2288" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2288" t="n">
+        <v>18</v>
+      </c>
+      <c r="I2288" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2288" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2288" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L2288" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M2288" t="n">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="2289">
+      <c r="A2289" t="n">
+        <v>614</v>
+      </c>
+      <c r="B2289" t="n">
+        <v>562</v>
+      </c>
+      <c r="C2289" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2289" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2289" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2289" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2289" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2289" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2289" t="n">
+        <v>103</v>
+      </c>
+      <c r="J2289" t="n">
+        <v>225</v>
+      </c>
+      <c r="K2289" t="n">
+        <v>226</v>
+      </c>
+      <c r="L2289" t="n">
+        <v>130</v>
+      </c>
+      <c r="M2289" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2290">
+      <c r="A2290" t="n">
+        <v>614</v>
+      </c>
+      <c r="B2290" t="n">
+        <v>563</v>
+      </c>
+      <c r="C2290" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2290" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2290" t="n">
+        <v>13</v>
+      </c>
+      <c r="F2290" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2290" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2290" t="n">
+        <v>31</v>
+      </c>
+      <c r="I2290" t="n">
+        <v>104</v>
+      </c>
+      <c r="J2290" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="K2290" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="L2290" t="n">
+        <v>190</v>
+      </c>
+      <c r="M2290" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="2291">
+      <c r="A2291" t="n">
+        <v>614</v>
+      </c>
+      <c r="B2291" t="n">
+        <v>564</v>
+      </c>
+      <c r="C2291" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2291" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2291" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2291" t="n">
+        <v>38</v>
+      </c>
+      <c r="G2291" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2291" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2291" t="n">
+        <v>118</v>
+      </c>
+      <c r="J2291" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2291" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2291" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M2291" t="n">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="2292">
+      <c r="A2292" t="n">
+        <v>615</v>
+      </c>
+      <c r="B2292" t="n">
+        <v>571</v>
+      </c>
+      <c r="C2292" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2292" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2292" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2292" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2292" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2292" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2292" t="n">
+        <v>108</v>
+      </c>
+      <c r="J2292" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K2292" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2292" t="n">
+        <v>-120</v>
+      </c>
+      <c r="M2292" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2293">
+      <c r="A2293" t="n">
+        <v>615</v>
+      </c>
+      <c r="B2293" t="n">
+        <v>572</v>
+      </c>
+      <c r="C2293" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2293" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2293" t="n">
+        <v>15</v>
+      </c>
+      <c r="F2293" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2293" t="n">
+        <v>38</v>
+      </c>
+      <c r="H2293" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2293" t="n">
+        <v>114</v>
+      </c>
+      <c r="J2293" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="K2293" t="n">
+        <v>222</v>
+      </c>
+      <c r="L2293" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2293" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2294">
+      <c r="A2294" t="n">
+        <v>616</v>
+      </c>
+      <c r="B2294" t="n">
+        <v>581</v>
+      </c>
+      <c r="C2294" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2294" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2294" t="n">
+        <v>24</v>
+      </c>
+      <c r="F2294" t="n">
+        <v>16</v>
+      </c>
+      <c r="G2294" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2294" t="n">
+        <v>40</v>
+      </c>
+      <c r="I2294" t="n">
+        <v>109</v>
+      </c>
+      <c r="J2294" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="K2294" t="n">
+        <v>224</v>
+      </c>
+      <c r="L2294" t="n">
+        <v>250</v>
+      </c>
+      <c r="M2294" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2295">
+      <c r="A2295" t="n">
+        <v>616</v>
+      </c>
+      <c r="B2295" t="n">
+        <v>582</v>
+      </c>
+      <c r="C2295" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2295" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2295" t="n">
+        <v>38</v>
+      </c>
+      <c r="F2295" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2295" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2295" t="n">
+        <v>19</v>
+      </c>
+      <c r="I2295" t="n">
+        <v>106</v>
+      </c>
+      <c r="J2295" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K2295" t="n">
+        <v>7</v>
+      </c>
+      <c r="L2295" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M2295" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2296">
+      <c r="A2296" t="n">
+        <v>616</v>
+      </c>
+      <c r="B2296" t="n">
+        <v>583</v>
+      </c>
+      <c r="C2296" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2296" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2296" t="n">
+        <v>36</v>
+      </c>
+      <c r="F2296" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2296" t="n">
+        <v>32</v>
+      </c>
+      <c r="H2296" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2296" t="n">
+        <v>119</v>
+      </c>
+      <c r="J2296" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="K2296" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="L2296" t="n">
+        <v>310</v>
+      </c>
+      <c r="M2296" t="n">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" t="n">
+        <v>616</v>
+      </c>
+      <c r="B2297" t="n">
+        <v>584</v>
+      </c>
+      <c r="C2297" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2297" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2297" t="n">
+        <v>37</v>
+      </c>
+      <c r="F2297" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2297" t="n">
+        <v>18</v>
+      </c>
+      <c r="H2297" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2297" t="n">
+        <v>111</v>
+      </c>
+      <c r="J2297" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K2297" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L2297" t="n">
+        <v>-370</v>
+      </c>
+      <c r="M2297" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="2298">
+      <c r="A2298" t="n">
+        <v>617</v>
+      </c>
+      <c r="B2298" t="n">
+        <v>501</v>
+      </c>
+      <c r="C2298" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2298" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2298" t="n">
+        <v>19</v>
+      </c>
+      <c r="F2298" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2298" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2298" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2298" t="n">
+        <v>89</v>
+      </c>
+      <c r="J2298" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="K2298" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="L2298" t="n">
+        <v>175</v>
+      </c>
+      <c r="M2298" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2299">
+      <c r="A2299" t="n">
+        <v>617</v>
+      </c>
+      <c r="B2299" t="n">
+        <v>502</v>
+      </c>
+      <c r="C2299" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2299" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2299" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2299" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2299" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2299" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2299" t="n">
+        <v>104</v>
+      </c>
+      <c r="J2299" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2299" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2299" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M2299" t="n">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="2300">
+      <c r="A2300" t="n">
+        <v>618</v>
+      </c>
+      <c r="B2300" t="n">
+        <v>511</v>
+      </c>
+      <c r="C2300" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2300" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2300" t="n">
+        <v>22</v>
+      </c>
+      <c r="F2300" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2300" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2300" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2300" t="n">
+        <v>104</v>
+      </c>
+      <c r="J2300" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2300" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2300" t="n">
+        <v>175</v>
+      </c>
+      <c r="M2300" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2301">
+      <c r="A2301" t="n">
+        <v>618</v>
+      </c>
+      <c r="B2301" t="n">
+        <v>512</v>
+      </c>
+      <c r="C2301" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2301" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2301" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2301" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2301" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2301" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2301" t="n">
+        <v>99</v>
+      </c>
+      <c r="J2301" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="K2301" t="n">
+        <v>223.5</v>
+      </c>
+      <c r="L2301" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M2301" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2302">
+      <c r="A2302" t="n">
+        <v>618</v>
+      </c>
+      <c r="B2302" t="n">
+        <v>513</v>
+      </c>
+      <c r="C2302" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2302" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E2302" t="n">
+        <v>33</v>
+      </c>
+      <c r="F2302" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2302" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2302" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2302" t="n">
+        <v>119</v>
+      </c>
+      <c r="J2302" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2302" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L2302" t="n">
+        <v>-155</v>
+      </c>
+      <c r="M2302" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2303">
+      <c r="A2303" t="n">
+        <v>618</v>
+      </c>
+      <c r="B2303" t="n">
+        <v>514</v>
+      </c>
+      <c r="C2303" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2303" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2303" t="n">
+        <v>31</v>
+      </c>
+      <c r="F2303" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2303" t="n">
+        <v>41</v>
+      </c>
+      <c r="H2303" t="n">
+        <v>40</v>
+      </c>
+      <c r="I2303" t="n">
+        <v>131</v>
+      </c>
+      <c r="J2303" t="n">
+        <v>218.5</v>
+      </c>
+      <c r="K2303" t="n">
+        <v>221</v>
+      </c>
+      <c r="L2303" t="n">
+        <v>135</v>
+      </c>
+      <c r="M2303" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="2304">
+      <c r="A2304" t="n">
+        <v>619</v>
+      </c>
+      <c r="B2304" t="n">
+        <v>521</v>
+      </c>
+      <c r="C2304" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2304" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2304" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2304" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2304" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2304" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2304" t="n">
+        <v>115</v>
+      </c>
+      <c r="J2304" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2304" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="L2304" t="n">
+        <v>-145</v>
+      </c>
+      <c r="M2304" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2305">
+      <c r="A2305" t="n">
+        <v>619</v>
+      </c>
+      <c r="B2305" t="n">
+        <v>522</v>
+      </c>
+      <c r="C2305" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2305" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E2305" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2305" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2305" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2305" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2305" t="n">
+        <v>111</v>
+      </c>
+      <c r="J2305" t="n">
+        <v>216.5</v>
+      </c>
+      <c r="K2305" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2305" t="n">
+        <v>125</v>
+      </c>
+      <c r="M2305" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2306">
+      <c r="A2306" t="n">
+        <v>620</v>
+      </c>
+      <c r="B2306" t="n">
+        <v>533</v>
+      </c>
+      <c r="C2306" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2306" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2306" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2306" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2306" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2306" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2306" t="n">
+        <v>103</v>
+      </c>
+      <c r="J2306" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="K2306" t="n">
+        <v>216</v>
+      </c>
+      <c r="L2306" t="n">
+        <v>240</v>
+      </c>
+      <c r="M2306" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2307">
+      <c r="A2307" t="n">
+        <v>620</v>
+      </c>
+      <c r="B2307" t="n">
+        <v>534</v>
+      </c>
+      <c r="C2307" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2307" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E2307" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2307" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2307" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2307" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2307" t="n">
+        <v>96</v>
+      </c>
+      <c r="J2307" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K2307" t="n">
+        <v>7</v>
+      </c>
+      <c r="L2307" t="n">
+        <v>-280</v>
+      </c>
+      <c r="M2307" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="2308">
+      <c r="A2308" t="n">
+        <v>620</v>
+      </c>
+      <c r="B2308" t="n">
+        <v>535</v>
+      </c>
+      <c r="C2308" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2308" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2308" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2308" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2308" t="n">
+        <v>39</v>
+      </c>
+      <c r="H2308" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2308" t="n">
+        <v>114</v>
+      </c>
+      <c r="J2308" t="n">
+        <v>221.5</v>
+      </c>
+      <c r="K2308" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="L2308" t="n">
+        <v>150</v>
+      </c>
+      <c r="M2308" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2309">
+      <c r="A2309" t="n">
+        <v>620</v>
+      </c>
+      <c r="B2309" t="n">
+        <v>536</v>
+      </c>
+      <c r="C2309" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2309" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2309" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2309" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2309" t="n">
+        <v>36</v>
+      </c>
+      <c r="H2309" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2309" t="n">
+        <v>120</v>
+      </c>
+      <c r="J2309" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2309" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2309" t="n">
+        <v>-170</v>
+      </c>
+      <c r="M2309" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="2310">
+      <c r="A2310" t="n">
+        <v>622</v>
+      </c>
+      <c r="B2310" t="n">
+        <v>551</v>
+      </c>
+      <c r="C2310" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2310" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2310" t="n">
+        <v>22</v>
+      </c>
+      <c r="F2310" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2310" t="n">
+        <v>24</v>
+      </c>
+      <c r="H2310" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2310" t="n">
+        <v>103</v>
+      </c>
+      <c r="J2310" t="n">
+        <v>224</v>
+      </c>
+      <c r="K2310" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="L2310" t="n">
+        <v>165</v>
+      </c>
+      <c r="M2310" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2311">
+      <c r="A2311" t="n">
+        <v>622</v>
+      </c>
+      <c r="B2311" t="n">
+        <v>552</v>
+      </c>
+      <c r="C2311" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2311" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2311" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2311" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2311" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2311" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2311" t="n">
+        <v>104</v>
+      </c>
+      <c r="J2311" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2311" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2311" t="n">
+        <v>-185</v>
+      </c>
+      <c r="M2311" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2312">
+      <c r="A2312" t="n">
+        <v>623</v>
+      </c>
+      <c r="B2312" t="n">
+        <v>561</v>
+      </c>
+      <c r="C2312" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2312" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2312" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2312" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2312" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2312" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2312" t="n">
+        <v>116</v>
+      </c>
+      <c r="J2312" t="n">
+        <v>227.5</v>
+      </c>
+      <c r="K2312" t="n">
+        <v>225</v>
+      </c>
+      <c r="L2312" t="n">
+        <v>300</v>
+      </c>
+      <c r="M2312" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2313">
+      <c r="A2313" t="n">
+        <v>623</v>
+      </c>
+      <c r="B2313" t="n">
+        <v>562</v>
+      </c>
+      <c r="C2313" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2313" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2313" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2313" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2313" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2313" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2313" t="n">
+        <v>113</v>
+      </c>
+      <c r="J2313" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K2313" t="n">
+        <v>8</v>
+      </c>
+      <c r="L2313" t="n">
+        <v>-360</v>
+      </c>
+      <c r="M2313" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2314">
+      <c r="A2314" t="n">
+        <v>624</v>
+      </c>
+      <c r="B2314" t="n">
+        <v>571</v>
+      </c>
+      <c r="C2314" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2314" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2314" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2314" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2314" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2314" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2314" t="n">
+        <v>92</v>
+      </c>
+      <c r="J2314" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2314" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2314" t="n">
+        <v>-115</v>
+      </c>
+      <c r="M2314" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2315">
+      <c r="A2315" t="n">
+        <v>624</v>
+      </c>
+      <c r="B2315" t="n">
+        <v>572</v>
+      </c>
+      <c r="C2315" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2315" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2315" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2315" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2315" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2315" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2315" t="n">
+        <v>106</v>
+      </c>
+      <c r="J2315" t="n">
+        <v>218.5</v>
+      </c>
+      <c r="K2315" t="n">
+        <v>221</v>
+      </c>
+      <c r="L2315" t="n">
+        <v>-105</v>
+      </c>
+      <c r="M2315" t="n">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="2316">
+      <c r="A2316" t="n">
+        <v>625</v>
+      </c>
+      <c r="B2316" t="n">
+        <v>581</v>
+      </c>
+      <c r="C2316" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2316" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2316" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2316" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2316" t="n">
+        <v>18</v>
+      </c>
+      <c r="H2316" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2316" t="n">
+        <v>91</v>
+      </c>
+      <c r="J2316" t="n">
+        <v>226.5</v>
+      </c>
+      <c r="K2316" t="n">
+        <v>226</v>
+      </c>
+      <c r="L2316" t="n">
+        <v>310</v>
+      </c>
+      <c r="M2316" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="2317">
+      <c r="A2317" t="n">
+        <v>625</v>
+      </c>
+      <c r="B2317" t="n">
+        <v>582</v>
+      </c>
+      <c r="C2317" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2317" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2317" t="n">
+        <v>34</v>
+      </c>
+      <c r="F2317" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2317" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2317" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2317" t="n">
+        <v>125</v>
+      </c>
+      <c r="J2317" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K2317" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L2317" t="n">
+        <v>-370</v>
+      </c>
+      <c r="M2317" t="n">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="2318">
+      <c r="A2318" t="n">
+        <v>626</v>
+      </c>
+      <c r="B2318" t="n">
+        <v>591</v>
+      </c>
+      <c r="C2318" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2318" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2318" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2318" t="n">
+        <v>21</v>
+      </c>
+      <c r="G2318" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2318" t="n">
+        <v>15</v>
+      </c>
+      <c r="I2318" t="n">
+        <v>84</v>
+      </c>
+      <c r="J2318" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2318" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="L2318" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M2318" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="2319">
+      <c r="A2319" t="n">
+        <v>626</v>
+      </c>
+      <c r="B2319" t="n">
+        <v>592</v>
+      </c>
+      <c r="C2319" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2319" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2319" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2319" t="n">
+        <v>16</v>
+      </c>
+      <c r="G2319" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2319" t="n">
+        <v>14</v>
+      </c>
+      <c r="I2319" t="n">
+        <v>80</v>
+      </c>
+      <c r="J2319" t="n">
+        <v>220</v>
+      </c>
+      <c r="K2319" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L2319" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M2319" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2320">
+      <c r="A2320" t="n">
+        <v>627</v>
+      </c>
+      <c r="B2320" t="n">
+        <v>501</v>
+      </c>
+      <c r="C2320" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2320" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2320" t="n">
+        <v>27</v>
+      </c>
+      <c r="F2320" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2320" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2320" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2320" t="n">
+        <v>113</v>
+      </c>
+      <c r="J2320" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2320" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2320" t="n">
+        <v>-185</v>
+      </c>
+      <c r="M2320" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="2321">
+      <c r="A2321" t="n">
+        <v>627</v>
+      </c>
+      <c r="B2321" t="n">
+        <v>502</v>
+      </c>
+      <c r="C2321" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2321" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2321" t="n">
+        <v>32</v>
+      </c>
+      <c r="F2321" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2321" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2321" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2321" t="n">
+        <v>102</v>
+      </c>
+      <c r="J2321" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="K2321" t="n">
+        <v>224</v>
+      </c>
+      <c r="L2321" t="n">
+        <v>165</v>
+      </c>
+      <c r="M2321" t="n">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="2322">
+      <c r="A2322" t="n">
+        <v>628</v>
+      </c>
+      <c r="B2322" t="n">
+        <v>511</v>
+      </c>
+      <c r="C2322" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2322" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2322" t="n">
+        <v>36</v>
+      </c>
+      <c r="F2322" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2322" t="n">
+        <v>32</v>
+      </c>
+      <c r="H2322" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2322" t="n">
+        <v>116</v>
+      </c>
+      <c r="J2322" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K2322" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="L2322" t="n">
+        <v>240</v>
+      </c>
+      <c r="M2322" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2323">
+      <c r="A2323" t="n">
+        <v>628</v>
+      </c>
+      <c r="B2323" t="n">
+        <v>512</v>
+      </c>
+      <c r="C2323" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2323" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2323" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2323" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2323" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2323" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2323" t="n">
+        <v>102</v>
+      </c>
+      <c r="J2323" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2323" t="n">
+        <v>7</v>
+      </c>
+      <c r="L2323" t="n">
+        <v>-280</v>
+      </c>
+      <c r="M2323" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2324">
+      <c r="A2324" t="n">
+        <v>629</v>
+      </c>
+      <c r="B2324" t="n">
+        <v>521</v>
+      </c>
+      <c r="C2324" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2324" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2324" t="n">
+        <v>22</v>
+      </c>
+      <c r="F2324" t="n">
+        <v>16</v>
+      </c>
+      <c r="G2324" t="n">
+        <v>24</v>
+      </c>
+      <c r="H2324" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2324" t="n">
+        <v>88</v>
+      </c>
+      <c r="J2324" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2324" t="n">
+        <v>9</v>
+      </c>
+      <c r="L2324" t="n">
+        <v>-420</v>
+      </c>
+      <c r="M2324" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="2325">
+      <c r="A2325" t="n">
+        <v>629</v>
+      </c>
+      <c r="B2325" t="n">
+        <v>522</v>
+      </c>
+      <c r="C2325" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2325" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2325" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2325" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2325" t="n">
+        <v>36</v>
+      </c>
+      <c r="H2325" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2325" t="n">
+        <v>110</v>
+      </c>
+      <c r="J2325" t="n">
+        <v>221.5</v>
+      </c>
+      <c r="K2325" t="n">
+        <v>215</v>
+      </c>
+      <c r="L2325" t="n">
+        <v>350</v>
+      </c>
+      <c r="M2325" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2326">
+      <c r="A2326" t="n">
+        <v>630</v>
+      </c>
+      <c r="B2326" t="n">
+        <v>531</v>
+      </c>
+      <c r="C2326" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2326" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2326" t="n">
+        <v>33</v>
+      </c>
+      <c r="F2326" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2326" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2326" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2326" t="n">
+        <v>130</v>
+      </c>
+      <c r="J2326" t="n">
+        <v>215</v>
+      </c>
+      <c r="K2326" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2326" t="n">
+        <v>-115</v>
+      </c>
+      <c r="M2326" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="2327">
+      <c r="A2327" t="n">
+        <v>630</v>
+      </c>
+      <c r="B2327" t="n">
+        <v>532</v>
+      </c>
+      <c r="C2327" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2327" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E2327" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2327" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2327" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2327" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2327" t="n">
+        <v>103</v>
+      </c>
+      <c r="J2327" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2327" t="n">
+        <v>214.5</v>
+      </c>
+      <c r="L2327" t="n">
+        <v>-105</v>
+      </c>
+      <c r="M2327" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2328">
+      <c r="A2328" t="n">
+        <v>701</v>
+      </c>
+      <c r="B2328" t="n">
+        <v>541</v>
+      </c>
+      <c r="C2328" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2328" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2328" t="n">
+        <v>22</v>
+      </c>
+      <c r="F2328" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2328" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2328" t="n">
+        <v>34</v>
+      </c>
+      <c r="I2328" t="n">
+        <v>112</v>
+      </c>
+      <c r="J2328" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="K2328" t="n">
+        <v>213</v>
+      </c>
+      <c r="L2328" t="n">
+        <v>165</v>
+      </c>
+      <c r="M2328" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2329">
+      <c r="A2329" t="n">
+        <v>701</v>
+      </c>
+      <c r="B2329" t="n">
+        <v>542</v>
+      </c>
+      <c r="C2329" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2329" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2329" t="n">
+        <v>36</v>
+      </c>
+      <c r="F2329" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2329" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2329" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2329" t="n">
+        <v>123</v>
+      </c>
+      <c r="J2329" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2329" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2329" t="n">
+        <v>-185</v>
+      </c>
+      <c r="M2329" t="n">
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="2330">
+      <c r="A2330" t="n">
+        <v>703</v>
+      </c>
+      <c r="B2330" t="n">
+        <v>561</v>
+      </c>
+      <c r="C2330" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2330" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2330" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2330" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2330" t="n">
+        <v>44</v>
+      </c>
+      <c r="H2330" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2330" t="n">
+        <v>118</v>
+      </c>
+      <c r="J2330" t="n">
+        <v>215</v>
+      </c>
+      <c r="K2330" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="L2330" t="n">
+        <v>140</v>
+      </c>
+      <c r="M2330" t="n">
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="2331">
+      <c r="A2331" t="n">
+        <v>703</v>
+      </c>
+      <c r="B2331" t="n">
+        <v>562</v>
+      </c>
+      <c r="C2331" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2331" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E2331" t="n">
+        <v>24</v>
+      </c>
+      <c r="F2331" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2331" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2331" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2331" t="n">
+        <v>107</v>
+      </c>
+      <c r="J2331" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="K2331" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L2331" t="n">
+        <v>-160</v>
+      </c>
+      <c r="M2331" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2332">
+      <c r="A2332" t="n">
+        <v>706</v>
+      </c>
+      <c r="B2332" t="n">
+        <v>501</v>
+      </c>
+      <c r="C2332" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2332" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2332" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2332" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2332" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2332" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2332" t="n">
+        <v>105</v>
+      </c>
+      <c r="J2332" t="n">
+        <v>217</v>
+      </c>
+      <c r="K2332" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="L2332" t="n">
+        <v>190</v>
+      </c>
+      <c r="M2332" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2333">
+      <c r="A2333" t="n">
+        <v>706</v>
+      </c>
+      <c r="B2333" t="n">
+        <v>502</v>
+      </c>
+      <c r="C2333" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2333" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2333" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2333" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2333" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2333" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2333" t="n">
+        <v>118</v>
+      </c>
+      <c r="J2333" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K2333" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2333" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M2333" t="n">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="2334">
+      <c r="A2334" t="n">
+        <v>708</v>
+      </c>
+      <c r="B2334" t="n">
+        <v>503</v>
+      </c>
+      <c r="C2334" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2334" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2334" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2334" t="n">
+        <v>16</v>
+      </c>
+      <c r="G2334" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2334" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2334" t="n">
+        <v>108</v>
+      </c>
+      <c r="J2334" t="n">
+        <v>221</v>
+      </c>
+      <c r="K2334" t="n">
+        <v>221</v>
+      </c>
+      <c r="L2334" t="n">
+        <v>160</v>
+      </c>
+      <c r="M2334" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="2335">
+      <c r="A2335" t="n">
+        <v>708</v>
+      </c>
+      <c r="B2335" t="n">
+        <v>504</v>
+      </c>
+      <c r="C2335" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2335" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2335" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2335" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2335" t="n">
+        <v>32</v>
+      </c>
+      <c r="H2335" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2335" t="n">
+        <v>118</v>
+      </c>
+      <c r="J2335" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K2335" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2335" t="n">
+        <v>-180</v>
+      </c>
+      <c r="M2335" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2336">
+      <c r="A2336" t="n">
+        <v>711</v>
+      </c>
+      <c r="B2336" t="n">
+        <v>505</v>
+      </c>
+      <c r="C2336" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2336" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2336" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2336" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2336" t="n">
+        <v>31</v>
+      </c>
+      <c r="H2336" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2336" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2336" t="n">
+        <v>222</v>
+      </c>
+      <c r="K2336" t="n">
+        <v>220</v>
+      </c>
+      <c r="L2336" t="n">
+        <v>180</v>
+      </c>
+      <c r="M2336" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2337">
+      <c r="A2337" t="n">
+        <v>711</v>
+      </c>
+      <c r="B2337" t="n">
+        <v>506</v>
+      </c>
+      <c r="C2337" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2337" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2337" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2337" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2337" t="n">
+        <v>38</v>
+      </c>
+      <c r="H2337" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2337" t="n">
+        <v>120</v>
+      </c>
+      <c r="J2337" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2337" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2337" t="n">
+        <v>-210</v>
+      </c>
+      <c r="M2337" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2338">
+      <c r="A2338" t="n">
+        <v>714</v>
+      </c>
+      <c r="B2338" t="n">
+        <v>507</v>
+      </c>
+      <c r="C2338" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2338" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2338" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2338" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2338" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2338" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2338" t="n">
+        <v>103</v>
+      </c>
+      <c r="J2338" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="K2338" t="n">
+        <v>221</v>
+      </c>
+      <c r="L2338" t="n">
+        <v>170</v>
+      </c>
+      <c r="M2338" t="n">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="2339">
+      <c r="A2339" t="n">
+        <v>714</v>
+      </c>
+      <c r="B2339" t="n">
+        <v>508</v>
+      </c>
+      <c r="C2339" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2339" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2339" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2339" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2339" t="n">
+        <v>24</v>
+      </c>
+      <c r="H2339" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2339" t="n">
+        <v>109</v>
+      </c>
+      <c r="J2339" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K2339" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2339" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M2339" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2340">
+      <c r="A2340" t="n">
+        <v>717</v>
+      </c>
+      <c r="B2340" t="n">
+        <v>509</v>
+      </c>
+      <c r="C2340" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2340" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2340" t="n">
+        <v>21</v>
+      </c>
+      <c r="F2340" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2340" t="n">
+        <v>36</v>
+      </c>
+      <c r="H2340" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2340" t="n">
+        <v>123</v>
+      </c>
+      <c r="J2340" t="n">
+        <v>218.5</v>
+      </c>
+      <c r="K2340" t="n">
+        <v>220</v>
+      </c>
+      <c r="L2340" t="n">
+        <v>150</v>
+      </c>
+      <c r="M2340" t="n">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="2341">
+      <c r="A2341" t="n">
+        <v>717</v>
+      </c>
+      <c r="B2341" t="n">
+        <v>510</v>
+      </c>
+      <c r="C2341" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2341" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2341" t="n">
+        <v>37</v>
+      </c>
+      <c r="F2341" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2341" t="n">
+        <v>29</v>
+      </c>
+      <c r="H2341" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2341" t="n">
+        <v>119</v>
+      </c>
+      <c r="J2341" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2341" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2341" t="n">
+        <v>-170</v>
+      </c>
+      <c r="M2341" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2342">
+      <c r="A2342" t="n">
+        <v>720</v>
+      </c>
+      <c r="B2342" t="n">
+        <v>511</v>
+      </c>
+      <c r="C2342" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D2342" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E2342" t="n">
+        <v>16</v>
+      </c>
+      <c r="F2342" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2342" t="n">
+        <v>30</v>
+      </c>
+      <c r="H2342" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2342" t="n">
+        <v>98</v>
+      </c>
+      <c r="J2342" t="n">
+        <v>223</v>
+      </c>
+      <c r="K2342" t="n">
+        <v>221</v>
+      </c>
+      <c r="L2342" t="n">
+        <v>170</v>
+      </c>
+      <c r="M2342" t="n">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="2343">
+      <c r="A2343" t="n">
+        <v>720</v>
+      </c>
+      <c r="B2343" t="n">
+        <v>512</v>
+      </c>
+      <c r="C2343" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D2343" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E2343" t="n">
+        <v>29</v>
+      </c>
+      <c r="F2343" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2343" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2343" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2343" t="n">
+        <v>105</v>
+      </c>
+      <c r="J2343" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2343" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L2343" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M2343" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>